<commit_message>
Updated Excel File with Kitchen Files
</commit_message>
<xml_diff>
--- a/Ressential/Content/Todo List.xlsx
+++ b/Ressential/Content/Todo List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\FINAL_FYP\Ressential\Ressential\Ressential\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\Desktop\FYP Project\Ressential\Ressential\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2180B67D-1956-40A5-BB87-CA087672EEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_warehouse" sheetId="4" r:id="rId1"/>
@@ -23,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="156">
   <si>
     <t>Warehouse</t>
   </si>
@@ -102,12 +94,6 @@
     <t>Receive Stock</t>
   </si>
   <si>
-    <t>Sale</t>
-  </si>
-  <si>
-    <t>Sale Return</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -135,9 +121,6 @@
     <t>Chef View</t>
   </si>
   <si>
-    <t>Customer View</t>
-  </si>
-  <si>
     <t>Item Name</t>
   </si>
   <si>
@@ -234,12 +217,6 @@
     <t>IssueDate</t>
   </si>
   <si>
-    <t>tbl_issueItems</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Branch Code</t>
   </si>
   <si>
@@ -339,9 +316,6 @@
     <t>RequisitionDate</t>
   </si>
   <si>
-    <t>KitchenID</t>
-  </si>
-  <si>
     <t>tbl_requisitionItems</t>
   </si>
   <si>
@@ -349,12 +323,186 @@
   </si>
   <si>
     <t>ItemQuantity</t>
+  </si>
+  <si>
+    <t>Receive Stock =&gt; tbl already created in warehouse</t>
+  </si>
+  <si>
+    <t>PurchaseNo</t>
+  </si>
+  <si>
+    <t>IssueNo</t>
+  </si>
+  <si>
+    <t>tbl_issueRequisitions</t>
+  </si>
+  <si>
+    <t>ReferenceNo</t>
+  </si>
+  <si>
+    <t>Status =&gt; Pending/Settled/Partially Setteled</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Change Status</t>
+  </si>
+  <si>
+    <t>Return Stock Create =&gt; tbl_stockReturn</t>
+  </si>
+  <si>
+    <t>ReturnDate</t>
+  </si>
+  <si>
+    <t>ReturnNo</t>
+  </si>
+  <si>
+    <t>ReturnID</t>
+  </si>
+  <si>
+    <t>tbl_ReturnItems</t>
+  </si>
+  <si>
+    <t>Status =&gt; Pending/Settled</t>
+  </si>
+  <si>
+    <t>ConsumeID</t>
+  </si>
+  <si>
+    <t>ConsumeDate</t>
+  </si>
+  <si>
+    <t>tbl_ConsumeItems</t>
+  </si>
+  <si>
+    <t>ConsumeItemID</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Wastage Create =&gt; tbl_wastage</t>
+  </si>
+  <si>
+    <t>WastageID</t>
+  </si>
+  <si>
+    <t>Consume Create =&gt; tbl_consume</t>
+  </si>
+  <si>
+    <t>WastageDate</t>
+  </si>
+  <si>
+    <t>tbl_WastageItems</t>
+  </si>
+  <si>
+    <t>Category Create =&gt; tbl_category</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Product Create =&gt; tbl_product</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductImage</t>
+  </si>
+  <si>
+    <t>ProductPrice</t>
+  </si>
+  <si>
+    <t>tbl_productItems</t>
+  </si>
+  <si>
+    <t>WastageItemsID</t>
+  </si>
+  <si>
+    <t>ProductItemsID</t>
+  </si>
+  <si>
+    <t>ChefID</t>
+  </si>
+  <si>
+    <t>Desription</t>
+  </si>
+  <si>
+    <t>OrderNo</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>Order Return</t>
+  </si>
+  <si>
+    <t>Order Create =&gt; tbl_orders</t>
+  </si>
+  <si>
+    <t>tbl_orderProducts</t>
+  </si>
+  <si>
+    <t>OrderProductID</t>
+  </si>
+  <si>
+    <t>ProductQuantity</t>
+  </si>
+  <si>
+    <t>Order Return Create =&gt; tbl_orderReturn</t>
+  </si>
+  <si>
+    <t>OrderReturnID</t>
+  </si>
+  <si>
+    <t>OrderReturnDate</t>
+  </si>
+  <si>
+    <t>Orders View</t>
+  </si>
+  <si>
+    <t>tbl_orderReturnProducts</t>
+  </si>
+  <si>
+    <t>OrderReturnProductID</t>
+  </si>
+  <si>
+    <t>Order No</t>
+  </si>
+  <si>
+    <t>EstimatedTime</t>
+  </si>
+  <si>
+    <t>Product Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,16 +579,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,388 +904,389 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="K12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L5" t="s">
-        <v>90</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>91</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" t="s">
-        <v>92</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="N9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
+      <c r="H14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1143,175 +1294,175 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>7</v>
       </c>
@@ -1322,71 +1473,454 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
+    <col min="16" max="16" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" customWidth="1"/>
+    <col min="20" max="20" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" t="s">
+        <v>147</v>
+      </c>
+      <c r="V1" t="s">
+        <v>150</v>
+      </c>
+      <c r="X1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P2" t="s">
+        <v>137</v>
+      </c>
+      <c r="S2" t="s">
+        <v>148</v>
+      </c>
+      <c r="V2" t="s">
+        <v>153</v>
+      </c>
+      <c r="X2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V3" t="s">
+        <v>154</v>
+      </c>
+      <c r="X3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" t="s">
+        <v>137</v>
+      </c>
+      <c r="V4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P6" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s">
+        <v>132</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P7" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" t="s">
+        <v>59</v>
+      </c>
+      <c r="T7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N8" t="s">
+        <v>131</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>137</v>
+      </c>
+      <c r="T8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N9" t="s">
+        <v>133</v>
+      </c>
+      <c r="P9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>127</v>
+      </c>
+      <c r="T9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>146</v>
+      </c>
+      <c r="T10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="N11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1395,170 +1929,168 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>7</v>
       </c>
@@ -1569,51 +2101,51 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>